<commit_message>
feat: Add Nu, Inter, and XP bank mappings, adjust Excel header reading, include new historical data, and introduce data inspection scripts.
</commit_message>
<xml_diff>
--- a/multiplos.xlsx
+++ b/multiplos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Python\Balancetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306915AC-D1FF-4C7D-8C33-E4F97D1E99CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109215BF-2585-4E35-BE71-BEFF2A56B9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{44D3D71F-7463-4A62-9654-FA7E03EB3154}"/>
+    <workbookView xWindow="-23940" yWindow="510" windowWidth="20610" windowHeight="14790" xr2:uid="{44D3D71F-7463-4A62-9654-FA7E03EB3154}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="337">
   <si>
     <t>Papel</t>
   </si>
@@ -1023,6 +1023,33 @@
   </si>
   <si>
     <t>618,63</t>
+  </si>
+  <si>
+    <t>INBR</t>
+  </si>
+  <si>
+    <t>ROXO</t>
+  </si>
+  <si>
+    <t>XPBR</t>
+  </si>
+  <si>
+    <t>31,8</t>
+  </si>
+  <si>
+    <t>9,97</t>
+  </si>
+  <si>
+    <t>16,0</t>
+  </si>
+  <si>
+    <t>0,97%</t>
+  </si>
+  <si>
+    <t>1,07%</t>
+  </si>
+  <si>
+    <t>0,0%</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1085,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1394,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66605C28-1A55-42D4-91AE-2F33FF1E66D3}">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,6 +3771,39 @@
         <v>28</v>
       </c>
     </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>328</v>
+      </c>
+      <c r="C37" t="s">
+        <v>333</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>329</v>
+      </c>
+      <c r="C38" t="s">
+        <v>331</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>330</v>
+      </c>
+      <c r="C39" t="s">
+        <v>332</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>